<commit_message>
se areglo el mensaje a telegram
</commit_message>
<xml_diff>
--- a/titulos_enviados_18-02-2025.xlsx
+++ b/titulos_enviados_18-02-2025.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A42"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,6 +447,286 @@
         </is>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Alienware Headset Inalámbrico, Blanco</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Bulova Winston C4844 - Reloj de Pared (1 Unidad), Color Plateado.</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>TOPLIVING Silla de Oficina Tipo Gerencial con Cabecera Ajustable Base Metálica para Home Office Silla, con Base Giratoria, Altura Regulable, Color Gris</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Simple Wisdom Librero de 5 Capas, Librero Organizador, Trapezoidal Librero Minimalista, Estante Organizador de Uso Multiescenario Adecuado para Sala de Estar, Oficina, Dormitorio, Cocina, Baño（Negro）</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Tent SUNDOME</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Lenovo Laptop Gaming LOQ 15IAX9E 15.6 Pulgadas Intel Core i5-12450HX 8GB 512 GB SSD RTX3050 de 8 núcleos, Windows 11 Home Color Luna Grey</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Bulova Clocks Precise Connect - Reloj de Pared C5001, 12.5 Pulgadas, Plata Mate y Azul</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>UGREEN Cable USB Micro Nylon Trenzado Rápido Cargador Compatible con Galaxy S7 S6 Edge S5 Nota 5, Xiaomi, Huawei, HTC, Oneplus, LG, E lectores, 1M</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Hyperkin Xenon Wired Controller (Black) For Xbox Series X|S/Xbox One/Windows 10|11</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Amazon Basics - Juego de sábanas de microfibra ligera y súper suave de fácil cuidado con bolsillos de 14 pulgadas de profundidad, individual, color crema</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>CRAFTSMAN Batería de Iones de Litio V20, 4.0 amperios Hora (CMCB204)</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>Bulova Clocks C4834 Luxfer Prism - Reloj de Pared Inspirado en Frank Lloyd Wright de 14 Pulgadas</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>Ernie Ball Earthwood Medium - Cuerdas para guitarra acústica de 12 cuerdas, bronce 80/20, calibre 11-28</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Anker 20W Hielo Cargador Rápido, Control de Temperatura Avanzado, Diseño Compacto 25% Más Pequeño, Compatible con iPhone y Samsung y Otros Dispositivos, USB C Tipo, 2 Colores</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>EASYTAO Tira Led Neón 5M 600 LED, IP65 Impermeable, Luces LED Flexible de Decoración para Adecuado TV, Salón, Dormitorio, Cuarto (Blanco Frío)</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>EASYTAO TV-308 Cámara de Seguridad Interior 2.5K, 4MP Cámara Alexa WiFi, iCSee y Tris Home App, Audio Bidireccional, Control Remoto, Detección de Movimiento, Visión Nocturna,Compatible con Alexa</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Logitech G Driving Force Shifter Palanca de Cambios para Volantes de Carreras G29, G920 y G923, 6 Velocidades, Marcha Atrás a Presion, Acero y Cuero - Negro</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Fabuloso Limpiador Multiusos Líquido Frescura Activa Lavanda 4 L. Antiviral y Antibacterial. Limpiador Desinfectante que Brinda 24 Horas de Frescura</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Fancy Pets Mueble/Rascador para Gato Tebas de 140 Centímetros de Altura</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>BYASKZIV Cargador Tipo C (1.5M)</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>Bluelander Mochila Cruzada Antirrobo Impermeable, Bolso de Pecho para Hombre, Bolso Bandolera con Puerto de Carga USB, Perfecta para Celular, Tablets, Actividades como Deportes, Compras</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>Raganet, Mochila Transportadora de Mascotas, Perros y Gatos, Back Pack Portátil para Mascota Pequeña (Máximo 7Kg) Medidas: Ancho 23cm Largo 33cm Altura 42cm (Color Negro)</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Nescafé Dolce Gusto Café en Cápsulas Diferentes Variedades 24 Cápsulas</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
+          <t>Feandrea Árbol para Gatos de 155 cm de Altura, 49 x 40 x 155 cm, Rascador para Gatos con 5 Postes, Felpa Multicapa, Blanco Crema MPCT192T01</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>HIKEO Hielera Térmica Extra Grande Impermeable (30 Litros/36 Latas), Mochila Térmica Portátil con Múltiples Compartimentos, Doble Pared a Prueba de Fugas para Hielo, Ideal para Camping, Picnic, Viajes</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>KitKat chocolate con leche 9 pz de 41.5gr</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>JBL Bar 300 Barra de Sonido 5.0 Wi-Fi/Bluetooth, 260W de Potencia, Dolby Atmos, Multibeam, con HDMI ARC - Negro</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Cama Matrimonial Base Y Cabecero de Almacenamiento con Luces Led 2 Salidas de CA y 2 USB,Con dos cajones extraíbles y Cabecero Plataforma Tapizada,Antideslizante,sin Ruido,Café Negro(Matrimonial/Full)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Tira Led Neon RGB 30M Luces Led Para Cuarto Exterior Flex Manguera Party Luz Lights Navidad Halloween Fiesta Lampara Habitacion Aesthetic Calida Leds Strip Home Decoracion 2 Rollos</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Deyidn Lámpara de tocador moderna de 2 Luces, oro lámparas Vidrio acrílico espejo LED luz ajustable moderna lámpara de pared escocesa (12W 4000k)</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Bluelander Radios de Comunicación Inalámbricos 2 Piezas, Walkie Talkie de Largo Alcance, Walkie Talkie Recargable con Base de Carga a Prueba de Agua, Radios Walkie Talkie para Guardia, Almacé, Camping</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>CYCROWN CycRun Bicicleta Electrica para Adultos, Moto Electrica con Potencia Máxima del Motor 1000W,Autonomía 70-90KM, Velocidad de 35KM/H, con 20" Neumático Moto Bicicleta de Montaña</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>MURAMASA Mesa De Centro para Sala Mesa De Centro Elevable con Compartimentos Ocultos y Estante De Almacenamiento Mueble para Sala con Estación De Carga Mesa Expandible Madera Negro</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Jimmy Choo Blossom, 3.3 Fluid Ounce</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Twinings, Twinings Pure Green Tea, 25 sobres de 2 gramos cada uno</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>120cm Credenza Recibidor con Tomacorrientes y Puertos USB,Mesa Consola de Entrada con 3 cajones y 3 Estantes,Muebles Mesa Consola para Sala,Recámara,Comedor,Soporte de TV,Barra de Café,Mesa de Sofá</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Funko Pop! Deluxe: Cuphead - The Devil In Chair - Figura de Vinilo Coleccionable - Idea de Regalo - Mercancia Oficial - Juguetes para Niños y Adultos - Video Games Fans - Muñeco para Coleccionistas</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>amiibo - Cat Mario - Super Mario Series</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>NESCAFÉ Dolce Gusto Cappuccino Skinny Light de 16 cápsulas</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>TURTLE BEACH RECON 70 BLUE CAMO MULTIPLATAFORMA</t>
+        </is>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>